<commit_message>
Added Hampsons code and data to get the figs in her 2015 paper
</commit_message>
<xml_diff>
--- a/Misc/BioEcon_Parameters Kotze 2017-10-16.xlsx
+++ b/Misc/BioEcon_Parameters Kotze 2017-10-16.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540"/>
+    <workbookView xWindow="10300" yWindow="460" windowWidth="18500" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1764,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>